<commit_message>
Added initial nowcast refactoring for new SQL tables (v0.20)
</commit_message>
<xml_diff>
--- a/modules/nowcast-model/nowcast-model-variables.xlsx
+++ b/modules/nowcast-model/nowcast-model-variables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\__Projects\econforecasting\modules\nowcast-model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA18C7D4-E636-4644-AC93-54940B9012BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FDD0509-7980-4C1E-A074-6F7BC78B0D25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{D5917CAB-2590-4FE1-9E2D-85810580C73C}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D5917CAB-2590-4FE1-9E2D-85810580C73C}"/>
   </bookViews>
   <sheets>
     <sheet name="variables" sheetId="12" r:id="rId1"/>
@@ -1481,83 +1481,30 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="43">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7D7D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="27">
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
         <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
         <name val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -1565,116 +1512,19 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7D7D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7D7D"/>
-        </patternFill>
-      </fill>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1735,42 +1585,17 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
         <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
+        <color theme="1"/>
         <name val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -1959,6 +1784,69 @@
         <scheme val="minor"/>
       </font>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7D7D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -1984,28 +1872,28 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{4AECC335-00AC-41E6-A3CA-F63691B92F69}" name="Table13279" displayName="Table13279" ref="A1:P96" totalsRowShown="0" headerRowDxfId="42" dataDxfId="41">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{4AECC335-00AC-41E6-A3CA-F63691B92F69}" name="Table13279" displayName="Table13279" ref="A1:P96" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
   <autoFilter ref="A1:P96" xr:uid="{EC6D9A60-7AF3-4545-B540-E43EAD70DF9B}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P96">
     <sortCondition ref="C1:C96"/>
   </sortState>
   <tableColumns count="16">
-    <tableColumn id="1" xr3:uid="{CA6DE630-5CD5-428A-8439-1A504496E546}" name="varname" dataDxfId="40"/>
-    <tableColumn id="9" xr3:uid="{62B19A4C-5AC5-4FBE-B49F-BB64B9102385}" name="fullname" dataDxfId="39"/>
-    <tableColumn id="15" xr3:uid="{D22B03C4-4AE3-48C2-A598-07C9E704433D}" name="dispgroup" dataDxfId="38"/>
-    <tableColumn id="24" xr3:uid="{FDF2E866-66A2-44DE-B360-10560B9D2BFE}" name="disporder" dataDxfId="37"/>
-    <tableColumn id="14" xr3:uid="{3D01EE11-409F-43C6-990A-ABD3232293C0}" name="release" dataDxfId="36"/>
-    <tableColumn id="12" xr3:uid="{814C0F50-71A5-4E9D-9399-51983A27304D}" name="units" dataDxfId="35"/>
-    <tableColumn id="4" xr3:uid="{4C279BEC-C29C-4B88-A87A-0A23F3DE4D9A}" name="st" dataDxfId="34"/>
-    <tableColumn id="13" xr3:uid="{4C82AECA-D40C-41E9-9170-45F127D67DD4}" name="d1" dataDxfId="33"/>
-    <tableColumn id="11" xr3:uid="{BCA31579-22E5-46AB-AC81-7237E8AE8CCD}" name="d2" dataDxfId="32"/>
-    <tableColumn id="7" xr3:uid="{3DB70CAB-2218-410A-943E-4B1A1CE99CE0}" name="hist_source" dataDxfId="28"/>
-    <tableColumn id="8" xr3:uid="{06E67E4A-E969-4950-94C0-63C7BE6000C6}" name="hist_source_key" dataDxfId="27"/>
-    <tableColumn id="10" xr3:uid="{295FC803-26EF-45A2-9731-0EF02F4740DB}" name="hist_source_freq" dataDxfId="26"/>
-    <tableColumn id="18" xr3:uid="{B33FA9FC-D56B-4B27-ABE5-74F23C66DD3F}" name="hist_source_transform" dataDxfId="9"/>
-    <tableColumn id="16" xr3:uid="{5323D81D-334B-41E1-9C57-FB97D32790FE}" name="nc_dfm_input" dataDxfId="31"/>
-    <tableColumn id="17" xr3:uid="{136836AD-D381-4336-9040-09625567FE1C}" name="nc_method" dataDxfId="30"/>
-    <tableColumn id="5" xr3:uid="{3F173539-12EB-41F3-B70E-7885DB3C4CE4}" name="nc_input_reason" dataDxfId="29"/>
+    <tableColumn id="1" xr3:uid="{CA6DE630-5CD5-428A-8439-1A504496E546}" name="varname" dataDxfId="15"/>
+    <tableColumn id="9" xr3:uid="{62B19A4C-5AC5-4FBE-B49F-BB64B9102385}" name="fullname" dataDxfId="14"/>
+    <tableColumn id="15" xr3:uid="{D22B03C4-4AE3-48C2-A598-07C9E704433D}" name="dispgroup" dataDxfId="13"/>
+    <tableColumn id="24" xr3:uid="{FDF2E866-66A2-44DE-B360-10560B9D2BFE}" name="disporder" dataDxfId="12"/>
+    <tableColumn id="14" xr3:uid="{3D01EE11-409F-43C6-990A-ABD3232293C0}" name="release" dataDxfId="11"/>
+    <tableColumn id="12" xr3:uid="{814C0F50-71A5-4E9D-9399-51983A27304D}" name="units" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{4C279BEC-C29C-4B88-A87A-0A23F3DE4D9A}" name="st" dataDxfId="9"/>
+    <tableColumn id="13" xr3:uid="{4C82AECA-D40C-41E9-9170-45F127D67DD4}" name="d1" dataDxfId="8"/>
+    <tableColumn id="11" xr3:uid="{BCA31579-22E5-46AB-AC81-7237E8AE8CCD}" name="d2" dataDxfId="7"/>
+    <tableColumn id="7" xr3:uid="{3DB70CAB-2218-410A-943E-4B1A1CE99CE0}" name="hist_source" dataDxfId="6"/>
+    <tableColumn id="8" xr3:uid="{06E67E4A-E969-4950-94C0-63C7BE6000C6}" name="hist_source_key" dataDxfId="5"/>
+    <tableColumn id="10" xr3:uid="{295FC803-26EF-45A2-9731-0EF02F4740DB}" name="hist_source_freq" dataDxfId="4"/>
+    <tableColumn id="18" xr3:uid="{B33FA9FC-D56B-4B27-ABE5-74F23C66DD3F}" name="hist_source_transform" dataDxfId="3"/>
+    <tableColumn id="16" xr3:uid="{5323D81D-334B-41E1-9C57-FB97D32790FE}" name="nc_dfm_input" dataDxfId="2"/>
+    <tableColumn id="17" xr3:uid="{136836AD-D381-4336-9040-09625567FE1C}" name="nc_method" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{3F173539-12EB-41F3-B70E-7885DB3C4CE4}" name="nc_input_reason" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2310,8 +2198,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C3B5527-644C-49DA-B440-BA66BC9FC6D2}">
   <dimension ref="A1:R96"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="J60" sqref="J60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5075,7 +4963,7 @@
         <v>189</v>
       </c>
       <c r="J58" s="4" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="K58" s="4" t="s">
         <v>41</v>
@@ -5124,7 +5012,7 @@
         <v>189</v>
       </c>
       <c r="J59" s="4" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="K59" s="4" t="s">
         <v>234</v>
@@ -6958,35 +6846,35 @@
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
   <conditionalFormatting sqref="N2:N96">
-    <cfRule type="expression" dxfId="8" priority="21">
+    <cfRule type="expression" dxfId="26" priority="21">
       <formula>AND($L2&lt;&gt;"d", $L2 &lt;&gt; "w", $L2&lt;&gt; "m")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O2:O96">
-    <cfRule type="cellIs" dxfId="7" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="9" operator="equal">
       <formula>"none"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="15" operator="equal">
       <formula>"dfm.q"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="16" operator="equal">
       <formula>"dfm.m"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="17" operator="equal">
       <formula>"calc"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:M96">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="1" operator="equal">
       <formula>"q"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="2" operator="equal">
       <formula>"m"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="3" operator="equal">
       <formula>"w"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="4" operator="equal">
       <formula>"d"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7002,7 +6890,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27F4DEC5-9444-4CCA-99A1-212DC975A3D7}">
   <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added nowcast improvements (v0.20)
</commit_message>
<xml_diff>
--- a/modules/nowcast-model/nowcast-model-variables.xlsx
+++ b/modules/nowcast-model/nowcast-model-variables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\__Projects\econforecasting\modules\nowcast-model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83467E9A-42B2-4820-94E1-570750F0E529}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DE5EA77-9B83-4D2C-A6E9-BBB3E5EA8911}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D5917CAB-2590-4FE1-9E2D-85810580C73C}"/>
   </bookViews>
@@ -2198,8 +2198,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C3B5527-644C-49DA-B440-BA66BC9FC6D2}">
   <dimension ref="A1:R96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="O36" sqref="O36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3883,7 +3883,7 @@
       </c>
       <c r="N35" s="5"/>
       <c r="O35" s="5" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="P35" s="6"/>
       <c r="R35" s="3"/>

</xml_diff>